<commit_message>
V2 - LIMPIADO - 13/07/2023
</commit_message>
<xml_diff>
--- a/El Oficinista/listcodancho.xlsx
+++ b/El Oficinista/listcodancho.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merche\Desktop\El Oficinista\El Oficinista\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Merche\Desktop\El Oficinista\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$CX$219</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$CX$220</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="215">
   <si>
     <t>PE-0500.000000</t>
   </si>
@@ -662,178 +662,16 @@
     <t>cod</t>
   </si>
   <si>
-    <t>2AJ</t>
-  </si>
-  <si>
-    <t>2CN</t>
-  </si>
-  <si>
-    <t>2EH</t>
-  </si>
-  <si>
-    <t>2DT</t>
-  </si>
-  <si>
-    <t>2AB</t>
-  </si>
-  <si>
-    <t>2BF</t>
-  </si>
-  <si>
-    <t>2CF</t>
-  </si>
-  <si>
-    <t>2DI</t>
-  </si>
-  <si>
-    <t>2BW</t>
-  </si>
-  <si>
-    <t>2CP</t>
-  </si>
-  <si>
-    <t>2EA</t>
-  </si>
-  <si>
-    <t>2BE</t>
-  </si>
-  <si>
-    <t>2HA</t>
-  </si>
-  <si>
-    <t>2AN</t>
-  </si>
-  <si>
-    <t>2DP</t>
-  </si>
-  <si>
-    <t>2AY</t>
-  </si>
-  <si>
-    <t>2EW</t>
-  </si>
-  <si>
-    <t>2BR</t>
-  </si>
-  <si>
-    <t>30K</t>
-  </si>
-  <si>
-    <t>2EJ</t>
-  </si>
-  <si>
-    <t>2CA</t>
-  </si>
-  <si>
-    <t>2CC</t>
-  </si>
-  <si>
-    <t>2CL</t>
-  </si>
-  <si>
-    <t>2BL</t>
-  </si>
-  <si>
-    <t>40N</t>
-  </si>
-  <si>
-    <t>2DO</t>
-  </si>
-  <si>
-    <t>2AZ</t>
-  </si>
-  <si>
-    <t>2BJ</t>
-  </si>
-  <si>
-    <t>2AQ</t>
-  </si>
-  <si>
-    <t>2FB</t>
-  </si>
-  <si>
-    <t>2FC</t>
-  </si>
-  <si>
-    <t>2BS</t>
-  </si>
-  <si>
-    <t>2BP</t>
-  </si>
-  <si>
-    <t>2FD</t>
-  </si>
-  <si>
-    <t>2EN</t>
-  </si>
-  <si>
-    <t>2BC</t>
-  </si>
-  <si>
-    <t>2CD</t>
-  </si>
-  <si>
-    <t>2AP</t>
-  </si>
-  <si>
-    <t>2CO</t>
-  </si>
-  <si>
-    <t>30W</t>
-  </si>
-  <si>
-    <t>2CS</t>
-  </si>
-  <si>
-    <t>2FF</t>
-  </si>
-  <si>
-    <t>2CE</t>
-  </si>
-  <si>
-    <t>2EF</t>
-  </si>
-  <si>
-    <t>2ED</t>
-  </si>
-  <si>
-    <t>2DW</t>
-  </si>
-  <si>
-    <t>2AL</t>
-  </si>
-  <si>
-    <t>2ET</t>
-  </si>
-  <si>
-    <t>2BN</t>
-  </si>
-  <si>
-    <t>RP-0050.X</t>
-  </si>
-  <si>
-    <t>ME-0150.0.F</t>
-  </si>
-  <si>
-    <t>TA.0450.0N0.080</t>
-  </si>
-  <si>
-    <t>PA-0500.0S000P</t>
-  </si>
-  <si>
-    <t>RE-0010.0</t>
-  </si>
-  <si>
-    <t>TP.0900.0N0.145</t>
-  </si>
-  <si>
     <t>MA-0830.0.F</t>
   </si>
   <si>
-    <t>378</t>
-  </si>
-  <si>
     <t>1620</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>25</t>
   </si>
 </sst>
 </file>
@@ -869,13 +707,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1156,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CX226"/>
+  <dimension ref="A1:CX220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="C226" sqref="C226"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1781,9 +1615,6 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2">
-        <v>221</v>
-      </c>
       <c r="C3" s="1">
         <v>2150</v>
       </c>
@@ -1805,6 +1636,15 @@
       <c r="K3" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM3" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS3" s="1" t="s">
         <v>209</v>
       </c>
@@ -1816,15 +1656,15 @@
       </c>
       <c r="BY3" s="1">
         <v>0</v>
+      </c>
+      <c r="CD3" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
-        <v>154</v>
-      </c>
       <c r="C4" s="1">
         <v>1700</v>
       </c>
@@ -1839,9 +1679,6 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
-        <v>202</v>
-      </c>
       <c r="C5" s="1">
         <v>2150</v>
       </c>
@@ -1863,6 +1700,15 @@
       <c r="K5" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH5" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK5" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM5" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS5" s="1" t="s">
         <v>209</v>
       </c>
@@ -1874,15 +1720,15 @@
       </c>
       <c r="BY5" s="1">
         <v>0</v>
+      </c>
+      <c r="CD5" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="C6" s="1">
         <v>2150</v>
       </c>
@@ -1904,6 +1750,15 @@
       <c r="K6" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK6" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM6" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS6" s="1" t="s">
         <v>209</v>
       </c>
@@ -1915,15 +1770,15 @@
       </c>
       <c r="BY6" s="1">
         <v>0</v>
+      </c>
+      <c r="CD6" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>212</v>
-      </c>
       <c r="C7" s="1">
         <v>2150</v>
       </c>
@@ -1945,6 +1800,15 @@
       <c r="K7" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH7" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM7" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS7" s="1" t="s">
         <v>209</v>
       </c>
@@ -1956,15 +1820,15 @@
       </c>
       <c r="BY7" s="1">
         <v>0</v>
+      </c>
+      <c r="CD7" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>107</v>
-      </c>
       <c r="C8" s="1">
         <v>1600</v>
       </c>
@@ -1982,9 +1846,6 @@
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>105</v>
-      </c>
       <c r="C9" s="1">
         <v>1600</v>
       </c>
@@ -1999,9 +1860,6 @@
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2">
-        <v>340</v>
-      </c>
       <c r="C10" s="1">
         <v>1620</v>
       </c>
@@ -2016,9 +1874,6 @@
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2">
-        <v>436</v>
-      </c>
       <c r="C11" s="1">
         <v>1635</v>
       </c>
@@ -2033,9 +1888,6 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2">
-        <v>414</v>
-      </c>
       <c r="C12" s="1">
         <v>1600</v>
       </c>
@@ -2050,9 +1902,6 @@
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2">
-        <v>439</v>
-      </c>
       <c r="C13" s="1">
         <v>1650</v>
       </c>
@@ -2067,9 +1916,6 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2">
-        <v>200</v>
-      </c>
       <c r="C14" s="1">
         <v>2150</v>
       </c>
@@ -2091,6 +1937,15 @@
       <c r="K14" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH14" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK14" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM14" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS14" s="1" t="s">
         <v>209</v>
       </c>
@@ -2102,15 +1957,15 @@
       </c>
       <c r="BY14" s="1">
         <v>0</v>
+      </c>
+      <c r="CD14" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="2">
-        <v>234</v>
-      </c>
       <c r="C15" s="1">
         <v>2150</v>
       </c>
@@ -2132,6 +1987,15 @@
       <c r="K15" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH15" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK15" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM15" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS15" s="1" t="s">
         <v>209</v>
       </c>
@@ -2143,15 +2007,15 @@
       </c>
       <c r="BY15" s="1">
         <v>0</v>
+      </c>
+      <c r="CD15" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:102" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2">
-        <v>194</v>
-      </c>
       <c r="C16" s="1">
         <v>1600</v>
       </c>
@@ -2162,13 +2026,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2">
-        <v>226</v>
-      </c>
       <c r="C17" s="1">
         <v>2150</v>
       </c>
@@ -2190,6 +2051,15 @@
       <c r="K17" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH17" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK17" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM17" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS17" s="1" t="s">
         <v>209</v>
       </c>
@@ -2202,14 +2072,14 @@
       <c r="BY17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD17" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2">
-        <v>223</v>
-      </c>
       <c r="C18" s="1">
         <v>2150</v>
       </c>
@@ -2231,6 +2101,15 @@
       <c r="K18" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM18" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS18" s="1" t="s">
         <v>209</v>
       </c>
@@ -2243,14 +2122,14 @@
       <c r="BY18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD18" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2">
-        <v>472</v>
-      </c>
       <c r="C19" s="1">
         <v>1630</v>
       </c>
@@ -2261,13 +2140,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="20" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="2">
-        <v>207</v>
-      </c>
       <c r="C20" s="1">
         <v>2150</v>
       </c>
@@ -2289,6 +2165,15 @@
       <c r="K20" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH20" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK20" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM20" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS20" s="1" t="s">
         <v>209</v>
       </c>
@@ -2301,14 +2186,14 @@
       <c r="BY20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD20" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="C21" s="1">
         <v>2150</v>
       </c>
@@ -2330,6 +2215,15 @@
       <c r="K21" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK21" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM21" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS21" s="1" t="s">
         <v>209</v>
       </c>
@@ -2342,14 +2236,14 @@
       <c r="BY21" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD21" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="22" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2">
-        <v>340</v>
-      </c>
       <c r="C22" s="1">
         <v>1620</v>
       </c>
@@ -2360,13 +2254,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="2">
-        <v>205</v>
-      </c>
       <c r="C23" s="1">
         <v>2150</v>
       </c>
@@ -2388,6 +2279,15 @@
       <c r="K23" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH23" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK23" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM23" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS23" s="1" t="s">
         <v>209</v>
       </c>
@@ -2400,14 +2300,14 @@
       <c r="BY23" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD23" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="24" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2">
-        <v>319</v>
-      </c>
       <c r="C24" s="1">
         <v>1600</v>
       </c>
@@ -2418,13 +2318,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="25" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="2">
-        <v>212</v>
-      </c>
       <c r="C25" s="1">
         <v>2150</v>
       </c>
@@ -2446,6 +2343,15 @@
       <c r="K25" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH25" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK25" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM25" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS25" s="1" t="s">
         <v>209</v>
       </c>
@@ -2458,14 +2364,14 @@
       <c r="BY25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD25" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="2">
-        <v>233</v>
-      </c>
       <c r="C26" s="1">
         <v>2150</v>
       </c>
@@ -2487,6 +2393,15 @@
       <c r="K26" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH26" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK26" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM26" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS26" s="1" t="s">
         <v>209</v>
       </c>
@@ -2499,14 +2414,14 @@
       <c r="BY26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD26" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="2">
-        <v>405</v>
-      </c>
       <c r="C27" s="1">
         <v>1630</v>
       </c>
@@ -2517,13 +2432,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="2">
-        <v>270</v>
-      </c>
       <c r="C28" s="1">
         <v>2150</v>
       </c>
@@ -2545,6 +2457,15 @@
       <c r="K28" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK28" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM28" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS28" s="1" t="s">
         <v>209</v>
       </c>
@@ -2557,14 +2478,14 @@
       <c r="BY28" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD28" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2">
-        <v>206</v>
-      </c>
       <c r="C29" s="1">
         <v>2150</v>
       </c>
@@ -2586,6 +2507,15 @@
       <c r="K29" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH29" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK29" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM29" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS29" s="1" t="s">
         <v>209</v>
       </c>
@@ -2598,14 +2528,14 @@
       <c r="BY29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD29" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="2">
-        <v>230</v>
-      </c>
       <c r="C30" s="1">
         <v>2150</v>
       </c>
@@ -2627,6 +2557,15 @@
       <c r="K30" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH30" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM30" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS30" s="1" t="s">
         <v>209</v>
       </c>
@@ -2639,14 +2578,14 @@
       <c r="BY30" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD30" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="2">
-        <v>232</v>
-      </c>
       <c r="C31" s="1">
         <v>2150</v>
       </c>
@@ -2668,6 +2607,15 @@
       <c r="K31" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH31" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM31" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS31" s="1" t="s">
         <v>209</v>
       </c>
@@ -2680,14 +2628,14 @@
       <c r="BY31" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD31" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2">
-        <v>237</v>
-      </c>
       <c r="C32" s="1">
         <v>2150</v>
       </c>
@@ -2709,6 +2657,15 @@
       <c r="K32" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK32" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM32" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS32" s="1" t="s">
         <v>209</v>
       </c>
@@ -2721,14 +2678,14 @@
       <c r="BY32" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD32" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="33" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="C33" s="1">
         <v>1600</v>
       </c>
@@ -2739,13 +2696,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="2">
-        <v>201</v>
-      </c>
       <c r="C34" s="1">
         <v>2150</v>
       </c>
@@ -2767,6 +2721,15 @@
       <c r="K34" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH34" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK34" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM34" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS34" s="1" t="s">
         <v>209</v>
       </c>
@@ -2779,14 +2742,14 @@
       <c r="BY34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD34" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="2">
-        <v>113</v>
-      </c>
       <c r="C35" s="1">
         <v>1600</v>
       </c>
@@ -2797,13 +2760,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="2">
-        <v>421</v>
-      </c>
       <c r="C36" s="1">
         <v>1600</v>
       </c>
@@ -2814,13 +2774,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="37" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="2">
-        <v>202</v>
-      </c>
       <c r="C37" s="1">
         <v>2150</v>
       </c>
@@ -2842,6 +2799,15 @@
       <c r="K37" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH37" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK37" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM37" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS37" s="1" t="s">
         <v>209</v>
       </c>
@@ -2854,14 +2820,14 @@
       <c r="BY37" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD37" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="C38" s="1">
         <v>750</v>
       </c>
@@ -2883,6 +2849,15 @@
       <c r="K38" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH38" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM38" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS38" s="1" t="s">
         <v>209</v>
       </c>
@@ -2895,14 +2870,14 @@
       <c r="BY38" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD38" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>215</v>
-      </c>
       <c r="C39" s="1">
         <v>2150</v>
       </c>
@@ -2924,6 +2899,15 @@
       <c r="K39" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK39" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM39" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS39" s="1" t="s">
         <v>209</v>
       </c>
@@ -2936,14 +2920,14 @@
       <c r="BY39" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD39" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="40" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="2">
-        <v>108</v>
-      </c>
       <c r="C40" s="1">
         <v>2000</v>
       </c>
@@ -2954,13 +2938,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="2">
-        <v>126</v>
-      </c>
       <c r="C41" s="1">
         <v>1600</v>
       </c>
@@ -2971,13 +2952,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="2">
-        <v>340</v>
-      </c>
       <c r="C42" s="1">
         <v>1600</v>
       </c>
@@ -2988,13 +2966,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="C43" s="1">
         <v>2150</v>
       </c>
@@ -3016,6 +2991,15 @@
       <c r="K43" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK43" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM43" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS43" s="1" t="s">
         <v>209</v>
       </c>
@@ -3028,14 +3012,14 @@
       <c r="BY43" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD43" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B44" s="2">
-        <v>506</v>
-      </c>
       <c r="C44" s="1">
         <v>1800</v>
       </c>
@@ -3046,13 +3030,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="2">
-        <v>340</v>
-      </c>
       <c r="C45" s="1">
         <v>1600</v>
       </c>
@@ -3063,13 +3044,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="2">
-        <v>109</v>
-      </c>
       <c r="C46" s="1">
         <v>2000</v>
       </c>
@@ -3080,13 +3058,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="47" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="2">
-        <v>131</v>
-      </c>
       <c r="C47" s="1">
         <v>1350</v>
       </c>
@@ -3097,13 +3072,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="48" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B48" s="2">
-        <v>214</v>
-      </c>
       <c r="C48" s="1">
         <v>2150</v>
       </c>
@@ -3125,6 +3097,15 @@
       <c r="K48" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH48" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM48" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS48" s="1" t="s">
         <v>209</v>
       </c>
@@ -3137,14 +3118,14 @@
       <c r="BY48" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD48" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="C49" s="1">
         <v>2150</v>
       </c>
@@ -3166,6 +3147,15 @@
       <c r="K49" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH49" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK49" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM49" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS49" s="1" t="s">
         <v>209</v>
       </c>
@@ -3178,14 +3168,14 @@
       <c r="BY49" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD49" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>218</v>
-      </c>
       <c r="C50" s="1">
         <v>2150</v>
       </c>
@@ -3207,6 +3197,15 @@
       <c r="K50" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH50" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK50" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM50" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS50" s="1" t="s">
         <v>209</v>
       </c>
@@ -3219,14 +3218,14 @@
       <c r="BY50" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD50" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="2">
-        <v>502</v>
-      </c>
       <c r="C51" s="1">
         <v>1800</v>
       </c>
@@ -3237,13 +3236,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="52" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B52" s="2">
-        <v>225</v>
-      </c>
       <c r="C52" s="1">
         <v>2150</v>
       </c>
@@ -3265,6 +3261,15 @@
       <c r="K52" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH52" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK52" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM52" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS52" s="1" t="s">
         <v>209</v>
       </c>
@@ -3277,14 +3282,14 @@
       <c r="BY52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD52" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="53" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B53" s="2">
-        <v>258</v>
-      </c>
       <c r="C53" s="1">
         <v>2100</v>
       </c>
@@ -3295,13 +3300,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B54" s="2">
-        <v>249</v>
-      </c>
       <c r="C54" s="1">
         <v>2150</v>
       </c>
@@ -3312,13 +3314,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="55" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="C55" s="1">
         <v>2150</v>
       </c>
@@ -3340,6 +3339,15 @@
       <c r="K55" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH55" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK55" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM55" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS55" s="1" t="s">
         <v>209</v>
       </c>
@@ -3352,14 +3360,14 @@
       <c r="BY55" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD55" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="56" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="C56" s="1">
         <v>2150</v>
       </c>
@@ -3370,13 +3378,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B57" s="2">
-        <v>256</v>
-      </c>
       <c r="C57" s="1">
         <v>2150</v>
       </c>
@@ -3387,13 +3392,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="58" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="C58" s="1">
         <v>2150</v>
       </c>
@@ -3404,13 +3406,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="59" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="2">
-        <v>251</v>
-      </c>
       <c r="C59" s="1">
         <v>2150</v>
       </c>
@@ -3421,13 +3420,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="60" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="C60" s="1">
         <v>2150</v>
       </c>
@@ -3449,6 +3445,15 @@
       <c r="K60" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH60" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK60" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM60" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS60" s="1" t="s">
         <v>209</v>
       </c>
@@ -3461,14 +3466,14 @@
       <c r="BY60" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD60" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="C61" s="1">
         <v>2150</v>
       </c>
@@ -3490,6 +3495,15 @@
       <c r="K61" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH61" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK61" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM61" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS61" s="1" t="s">
         <v>209</v>
       </c>
@@ -3502,14 +3516,14 @@
       <c r="BY61" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD61" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="2">
-        <v>262</v>
-      </c>
       <c r="C62" s="1">
         <v>2100</v>
       </c>
@@ -3520,13 +3534,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="63" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>224</v>
-      </c>
       <c r="C63" s="1">
         <v>2150</v>
       </c>
@@ -3537,13 +3548,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="64" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="C64" s="1">
         <v>2150</v>
       </c>
@@ -3554,13 +3562,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="65" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B65" s="2">
-        <v>110</v>
-      </c>
       <c r="C65" s="1">
         <v>1600</v>
       </c>
@@ -3571,13 +3576,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="66" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B66" s="2">
-        <v>524</v>
-      </c>
       <c r="C66" s="1">
         <v>600</v>
       </c>
@@ -3588,13 +3590,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B67" s="2">
-        <v>525</v>
-      </c>
       <c r="C67" s="1">
         <v>600</v>
       </c>
@@ -3605,13 +3604,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="2">
-        <v>208</v>
-      </c>
       <c r="C68" s="1">
         <v>2150</v>
       </c>
@@ -3633,6 +3629,15 @@
       <c r="K68" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH68" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK68" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM68" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS68" s="1" t="s">
         <v>209</v>
       </c>
@@ -3645,14 +3650,14 @@
       <c r="BY68" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD68" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="C69" s="1">
         <v>2150</v>
       </c>
@@ -3663,13 +3668,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="70" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B70" s="2">
-        <v>222</v>
-      </c>
       <c r="C70" s="1">
         <v>2150</v>
       </c>
@@ -3691,6 +3693,15 @@
       <c r="K70" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH70" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK70" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM70" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS70" s="1" t="s">
         <v>209</v>
       </c>
@@ -3703,14 +3714,14 @@
       <c r="BY70" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD70" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="2">
-        <v>213</v>
-      </c>
       <c r="C71" s="1">
         <v>2150</v>
       </c>
@@ -3732,6 +3743,15 @@
       <c r="K71" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK71" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM71" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS71" s="1" t="s">
         <v>209</v>
       </c>
@@ -3744,14 +3764,14 @@
       <c r="BY71" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD71" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="2">
-        <v>610</v>
-      </c>
       <c r="C72" s="1">
         <v>1600</v>
       </c>
@@ -3762,13 +3782,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="73" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="2">
-        <v>151</v>
-      </c>
       <c r="C73" s="1">
         <v>1400</v>
       </c>
@@ -3779,13 +3796,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="C74" s="1">
         <v>2150</v>
       </c>
@@ -3807,6 +3821,15 @@
       <c r="K74" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH74" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK74" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM74" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS74" s="1" t="s">
         <v>209</v>
       </c>
@@ -3819,14 +3842,14 @@
       <c r="BY74" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD74" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="2">
-        <v>267</v>
-      </c>
       <c r="C75" s="1">
         <v>445</v>
       </c>
@@ -3837,13 +3860,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B76" s="2">
-        <v>231</v>
-      </c>
       <c r="C76" s="1">
         <v>2150</v>
       </c>
@@ -3865,6 +3885,15 @@
       <c r="K76" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH76" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK76" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM76" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS76" s="1" t="s">
         <v>209</v>
       </c>
@@ -3877,14 +3906,14 @@
       <c r="BY76" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD76" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B77" s="2">
-        <v>102</v>
-      </c>
       <c r="C77" s="1">
         <v>1700</v>
       </c>
@@ -3895,13 +3924,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="78" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B78" s="2">
-        <v>111</v>
-      </c>
       <c r="C78" s="1">
         <v>1700</v>
       </c>
@@ -3912,13 +3938,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="79" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B79" s="2">
-        <v>216</v>
-      </c>
       <c r="C79" s="1">
         <v>2150</v>
       </c>
@@ -3940,6 +3963,15 @@
       <c r="K79" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH79" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK79" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM79" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS79" s="1" t="s">
         <v>209</v>
       </c>
@@ -3952,14 +3984,14 @@
       <c r="BY79" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD79" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B80" s="2">
-        <v>209</v>
-      </c>
       <c r="C80" s="1">
         <v>2150</v>
       </c>
@@ -3981,6 +4013,15 @@
       <c r="K80" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH80" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK80" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM80" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS80" s="1" t="s">
         <v>209</v>
       </c>
@@ -3993,14 +4034,14 @@
       <c r="BY80" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD80" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="81" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="2">
-        <v>410</v>
-      </c>
       <c r="C81" s="1">
         <v>1880</v>
       </c>
@@ -4011,13 +4052,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="82" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B82" s="2">
-        <v>264</v>
-      </c>
       <c r="C82" s="1">
         <v>2150</v>
       </c>
@@ -4028,13 +4066,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="83" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B83" s="2">
-        <v>279</v>
-      </c>
       <c r="C83" s="1">
         <v>2150</v>
       </c>
@@ -4045,13 +4080,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="84" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="2">
-        <v>235</v>
-      </c>
       <c r="C84" s="1">
         <v>2150</v>
       </c>
@@ -4073,6 +4105,15 @@
       <c r="K84" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH84" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK84" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM84" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS84" s="1" t="s">
         <v>209</v>
       </c>
@@ -4085,14 +4126,14 @@
       <c r="BY84" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD84" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="85" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="2">
-        <v>380</v>
-      </c>
       <c r="C85" s="1">
         <v>1140</v>
       </c>
@@ -4103,13 +4144,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="86" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B86" s="2">
-        <v>484</v>
-      </c>
       <c r="C86" s="1">
         <v>2500</v>
       </c>
@@ -4120,13 +4158,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B87" s="2">
-        <v>437</v>
-      </c>
       <c r="C87" s="1">
         <v>1880</v>
       </c>
@@ -4137,13 +4172,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="88" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B88" s="2">
-        <v>377</v>
-      </c>
       <c r="C88" s="1">
         <v>1720</v>
       </c>
@@ -4154,13 +4186,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="89" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B89" s="2">
-        <v>112</v>
-      </c>
       <c r="C89" s="1">
         <v>2000</v>
       </c>
@@ -4171,13 +4200,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="90" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B90" s="2">
-        <v>282</v>
-      </c>
       <c r="C90" s="1">
         <v>2150</v>
       </c>
@@ -4199,6 +4225,15 @@
       <c r="K90" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH90" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK90" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM90" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS90" s="1" t="s">
         <v>209</v>
       </c>
@@ -4211,14 +4246,14 @@
       <c r="BY90" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD90" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="91" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B91" s="2">
-        <v>304</v>
-      </c>
       <c r="C91" s="1">
         <v>2560</v>
       </c>
@@ -4229,13 +4264,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="92" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B92" s="2">
-        <v>327</v>
-      </c>
       <c r="C92" s="1">
         <v>1190</v>
       </c>
@@ -4246,13 +4278,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B93" s="2">
-        <v>207</v>
-      </c>
       <c r="C93" s="1">
         <v>2150</v>
       </c>
@@ -4274,6 +4303,15 @@
       <c r="K93" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH93" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK93" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM93" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS93" s="1" t="s">
         <v>209</v>
       </c>
@@ -4286,14 +4324,14 @@
       <c r="BY93" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD93" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="94" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B94" s="2">
-        <v>403</v>
-      </c>
       <c r="C94" s="1">
         <v>1600</v>
       </c>
@@ -4304,13 +4342,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="95" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B95" s="2">
-        <v>484</v>
-      </c>
       <c r="C95" s="1">
         <v>2520</v>
       </c>
@@ -4321,13 +4356,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="96" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>228</v>
-      </c>
       <c r="C96" s="1">
         <v>2150</v>
       </c>
@@ -4338,13 +4370,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="97" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B97" s="2">
-        <v>262</v>
-      </c>
       <c r="C97" s="1">
         <v>2150</v>
       </c>
@@ -4355,13 +4384,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="98" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B98" s="2">
-        <v>294</v>
-      </c>
       <c r="C98" s="1">
         <v>2150</v>
       </c>
@@ -4383,6 +4409,15 @@
       <c r="K98" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH98" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK98" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM98" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS98" s="1" t="s">
         <v>209</v>
       </c>
@@ -4395,14 +4430,14 @@
       <c r="BY98" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD98" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="99" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B99" s="2">
-        <v>428</v>
-      </c>
       <c r="C99" s="1">
         <v>1690</v>
       </c>
@@ -4413,13 +4448,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="100" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B100" s="2">
-        <v>125</v>
-      </c>
       <c r="C100" s="1">
         <v>1600</v>
       </c>
@@ -4430,13 +4462,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="101" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B101" s="2">
-        <v>492</v>
-      </c>
       <c r="C101" s="1">
         <v>1580</v>
       </c>
@@ -4447,13 +4476,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="102" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B102" s="2">
-        <v>257</v>
-      </c>
       <c r="C102" s="1">
         <v>2150</v>
       </c>
@@ -4464,13 +4490,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="103" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B103" s="2">
-        <v>300</v>
-      </c>
       <c r="K103" s="1" t="s">
         <v>209</v>
       </c>
@@ -4478,13 +4501,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="104" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B104" s="2">
-        <v>337</v>
-      </c>
       <c r="C104" s="1">
         <v>1700</v>
       </c>
@@ -4495,13 +4515,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="105" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B105" s="2">
-        <v>416</v>
-      </c>
       <c r="C105" s="1">
         <v>1230</v>
       </c>
@@ -4512,13 +4529,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="106" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B106" s="2">
-        <v>357</v>
-      </c>
       <c r="C106" s="1">
         <v>1140</v>
       </c>
@@ -4529,13 +4543,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B107" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="C107" s="1">
         <v>1190</v>
       </c>
@@ -4546,13 +4557,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B108" s="2">
-        <v>367</v>
-      </c>
       <c r="K108" s="1" t="s">
         <v>209</v>
       </c>
@@ -4560,13 +4568,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B109" s="2">
-        <v>373</v>
-      </c>
       <c r="C109" s="1">
         <v>1130</v>
       </c>
@@ -4577,13 +4582,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="110" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B110" s="2">
-        <v>363</v>
-      </c>
       <c r="C110" s="1">
         <v>1190</v>
       </c>
@@ -4594,13 +4596,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="111" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B111" s="2">
-        <v>137</v>
-      </c>
       <c r="K111" s="1" t="s">
         <v>209</v>
       </c>
@@ -4608,13 +4607,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="112" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B112" s="2">
-        <v>254</v>
-      </c>
       <c r="K112" s="1" t="s">
         <v>209</v>
       </c>
@@ -4622,13 +4618,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B113" s="2">
-        <v>249</v>
-      </c>
       <c r="C113" s="1">
         <v>2150</v>
       </c>
@@ -4639,13 +4632,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="114" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B114" s="2">
-        <v>158</v>
-      </c>
       <c r="C114" s="1">
         <v>1600</v>
       </c>
@@ -4656,13 +4646,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="115" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B115" s="2">
-        <v>206</v>
-      </c>
       <c r="C115" s="1">
         <v>2150</v>
       </c>
@@ -4684,6 +4671,15 @@
       <c r="K115" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH115" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK115" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM115" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS115" s="1" t="s">
         <v>209</v>
       </c>
@@ -4696,14 +4692,14 @@
       <c r="BY115" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD115" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="116" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B116" s="2">
-        <v>181</v>
-      </c>
       <c r="C116" s="1">
         <v>1650</v>
       </c>
@@ -4714,13 +4710,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="117" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="C117" s="1">
         <v>2150</v>
       </c>
@@ -4742,6 +4735,15 @@
       <c r="K117" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH117" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK117" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM117" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS117" s="1" t="s">
         <v>209</v>
       </c>
@@ -4754,14 +4756,14 @@
       <c r="BY117" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD117" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="118" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="C118" s="1">
         <v>2150</v>
       </c>
@@ -4772,13 +4774,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B119" s="2">
-        <v>454</v>
-      </c>
       <c r="C119" s="1">
         <v>1360</v>
       </c>
@@ -4789,13 +4788,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="C120" s="1">
         <v>2200</v>
       </c>
@@ -4806,13 +4802,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="121" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B121" s="2">
-        <v>239</v>
-      </c>
       <c r="C121" s="1">
         <v>2150</v>
       </c>
@@ -4834,6 +4827,15 @@
       <c r="K121" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH121" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK121" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM121" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS121" s="1" t="s">
         <v>209</v>
       </c>
@@ -4846,14 +4848,14 @@
       <c r="BY121" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD121" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="122" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B122" s="2">
-        <v>189</v>
-      </c>
       <c r="C122" s="1">
         <v>1650</v>
       </c>
@@ -4864,13 +4866,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B123" s="2">
-        <v>116</v>
-      </c>
       <c r="C123" s="1">
         <v>950</v>
       </c>
@@ -4881,13 +4880,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="124" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B124" s="2" t="s">
-        <v>232</v>
-      </c>
       <c r="C124" s="1">
         <v>2150</v>
       </c>
@@ -4898,13 +4894,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="125" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B125" s="2">
-        <v>267</v>
-      </c>
       <c r="C125" s="1">
         <v>1830</v>
       </c>
@@ -4915,13 +4908,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="126" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B126" s="2">
-        <v>292</v>
-      </c>
       <c r="C126" s="1">
         <v>2150</v>
       </c>
@@ -4932,13 +4922,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="127" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B127" s="2">
-        <v>108</v>
-      </c>
       <c r="C127" s="1">
         <v>2000</v>
       </c>
@@ -4949,13 +4936,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="128" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B128" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="C128" s="1">
         <v>2150</v>
       </c>
@@ -4977,6 +4961,15 @@
       <c r="K128" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH128" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK128" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM128" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS128" s="1" t="s">
         <v>209</v>
       </c>
@@ -4989,14 +4982,14 @@
       <c r="BY128" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD128" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="129" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B129" s="2">
-        <v>463</v>
-      </c>
       <c r="C129" s="1">
         <v>1650</v>
       </c>
@@ -5007,13 +5000,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="130" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B130" s="2">
-        <v>259</v>
-      </c>
       <c r="C130" s="1">
         <v>2100</v>
       </c>
@@ -5024,13 +5014,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="131" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B131" s="2">
-        <v>282</v>
-      </c>
       <c r="C131" s="1">
         <v>2150</v>
       </c>
@@ -5052,6 +5039,15 @@
       <c r="K131" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH131" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK131" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM131" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS131" s="1" t="s">
         <v>209</v>
       </c>
@@ -5064,14 +5060,14 @@
       <c r="BY131" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="132" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD131" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B132" s="2">
-        <v>447</v>
-      </c>
       <c r="C132" s="1">
         <v>1620</v>
       </c>
@@ -5082,13 +5078,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="133" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B133" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="C133" s="1">
         <v>2200</v>
       </c>
@@ -5110,6 +5103,15 @@
       <c r="K133" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH133" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK133" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM133" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS133" s="1" t="s">
         <v>209</v>
       </c>
@@ -5122,14 +5124,14 @@
       <c r="BY133" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD133" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="134" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B134" s="2">
-        <v>350</v>
-      </c>
       <c r="C134" s="1">
         <v>1600</v>
       </c>
@@ -5140,13 +5142,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="135" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>235</v>
-      </c>
       <c r="C135" s="1">
         <v>1140</v>
       </c>
@@ -5157,13 +5156,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="136" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B136" s="2">
-        <v>484</v>
-      </c>
       <c r="C136" s="1">
         <v>2520</v>
       </c>
@@ -5174,13 +5170,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="137" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="C137" s="1">
         <v>2150</v>
       </c>
@@ -5191,13 +5184,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="138" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B138" s="2">
-        <v>311</v>
-      </c>
       <c r="K138" s="1" t="s">
         <v>209</v>
       </c>
@@ -5205,13 +5195,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="139" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B139" s="2">
-        <v>242</v>
-      </c>
       <c r="C139" s="1">
         <v>2150</v>
       </c>
@@ -5222,13 +5209,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="140" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B140" s="2">
-        <v>291</v>
-      </c>
       <c r="C140" s="1">
         <v>2150</v>
       </c>
@@ -5239,13 +5223,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="141" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="C141" s="1">
         <v>2150</v>
       </c>
@@ -5256,13 +5237,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="142" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B142" s="2">
-        <v>128</v>
-      </c>
       <c r="C142" s="1">
         <v>1600</v>
       </c>
@@ -5273,13 +5251,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="143" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B143" s="2">
-        <v>266</v>
-      </c>
       <c r="C143" s="1">
         <v>2150</v>
       </c>
@@ -5290,13 +5265,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="144" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B144" s="2">
-        <v>356</v>
-      </c>
       <c r="C144" s="1">
         <v>1150</v>
       </c>
@@ -5307,13 +5279,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="145" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B145" s="2">
-        <v>337</v>
-      </c>
       <c r="C145" s="1">
         <v>1700</v>
       </c>
@@ -5324,13 +5293,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="146" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B146" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="C146" s="1">
         <v>2150</v>
       </c>
@@ -5341,13 +5307,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="147" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B147" s="2">
-        <v>401</v>
-      </c>
       <c r="C147" s="1">
         <v>1880</v>
       </c>
@@ -5358,13 +5321,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="148" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B148" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="C148" s="1">
         <v>2150</v>
       </c>
@@ -5386,6 +5346,15 @@
       <c r="K148" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH148" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK148" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM148" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS148" s="1" t="s">
         <v>209</v>
       </c>
@@ -5398,14 +5367,14 @@
       <c r="BY148" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="149" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD148" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="149" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B149" s="2">
-        <v>337</v>
-      </c>
       <c r="C149" s="1">
         <v>1700</v>
       </c>
@@ -5416,13 +5385,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="150" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="C150" s="1">
         <v>2150</v>
       </c>
@@ -5433,13 +5399,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="151" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B151" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="C151" s="1">
         <v>2150</v>
       </c>
@@ -5450,13 +5413,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="152" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B152" s="2">
-        <v>260</v>
-      </c>
       <c r="C152" s="1">
         <v>2150</v>
       </c>
@@ -5467,13 +5427,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="153" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B153" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="C153" s="1">
         <v>2150</v>
       </c>
@@ -5495,6 +5452,15 @@
       <c r="K153" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH153" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK153" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM153" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS153" s="1" t="s">
         <v>209</v>
       </c>
@@ -5507,14 +5473,14 @@
       <c r="BY153" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD153" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="154" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B154" s="2">
-        <v>268</v>
-      </c>
       <c r="C154" s="1">
         <v>2150</v>
       </c>
@@ -5525,13 +5491,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="155" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B155" s="2">
-        <v>481</v>
-      </c>
       <c r="C155" s="1">
         <v>1200</v>
       </c>
@@ -5542,13 +5505,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="156" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B156" s="2">
-        <v>336</v>
-      </c>
       <c r="C156" s="1">
         <v>1190</v>
       </c>
@@ -5559,13 +5519,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="157" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B157" s="2">
-        <v>651</v>
-      </c>
       <c r="C157" s="1">
         <v>1600</v>
       </c>
@@ -5576,13 +5533,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="158" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B158" s="2">
-        <v>802</v>
-      </c>
       <c r="C158" s="1">
         <v>1100</v>
       </c>
@@ -5593,13 +5547,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="159" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="C159" s="1">
         <v>2150</v>
       </c>
@@ -5610,13 +5561,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="160" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="C160" s="1">
         <v>2150</v>
       </c>
@@ -5638,6 +5586,15 @@
       <c r="K160" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH160" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK160" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM160" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS160" s="1" t="s">
         <v>209</v>
       </c>
@@ -5650,14 +5607,14 @@
       <c r="BY160" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD160" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="161" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="C161" s="1">
         <v>2150</v>
       </c>
@@ -5679,6 +5636,15 @@
       <c r="K161" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH161" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK161" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM161" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS161" s="1" t="s">
         <v>209</v>
       </c>
@@ -5691,14 +5657,14 @@
       <c r="BY161" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="162" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD161" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="162" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B162" s="2">
-        <v>115</v>
-      </c>
       <c r="C162" s="1">
         <v>1600</v>
       </c>
@@ -5709,13 +5675,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="163" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B163" s="2">
-        <v>305</v>
-      </c>
       <c r="C163" s="1">
         <v>1530</v>
       </c>
@@ -5726,13 +5689,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="164" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="C164" s="1">
         <v>2150</v>
       </c>
@@ -5754,6 +5714,15 @@
       <c r="K164" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH164" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK164" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM164" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS164" s="1" t="s">
         <v>209</v>
       </c>
@@ -5766,14 +5735,14 @@
       <c r="BY164" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD164" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="165" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B165" s="2">
-        <v>509</v>
-      </c>
       <c r="C165" s="1">
         <v>1800</v>
       </c>
@@ -5784,13 +5753,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="166" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B166" s="2">
-        <v>469</v>
-      </c>
       <c r="C166" s="1">
         <v>1800</v>
       </c>
@@ -5801,13 +5767,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="167" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B167" s="2">
-        <v>369</v>
-      </c>
       <c r="C167" s="1">
         <v>1190</v>
       </c>
@@ -5818,13 +5781,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="168" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B168" s="2">
-        <v>320</v>
-      </c>
       <c r="C168" s="1">
         <v>1450</v>
       </c>
@@ -5835,13 +5795,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="169" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B169" s="2">
-        <v>307</v>
-      </c>
       <c r="C169" s="1">
         <v>1190</v>
       </c>
@@ -5852,13 +5809,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="170" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B170" s="2">
-        <v>329</v>
-      </c>
       <c r="C170" s="1">
         <v>1640</v>
       </c>
@@ -5869,13 +5823,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="171" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B171" s="2">
-        <v>266</v>
-      </c>
       <c r="C171" s="1">
         <v>2150</v>
       </c>
@@ -5886,13 +5837,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="172" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B172" s="2">
-        <v>400</v>
-      </c>
       <c r="C172" s="1">
         <v>1570</v>
       </c>
@@ -5903,13 +5851,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="173" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B173" s="2">
-        <v>406</v>
-      </c>
       <c r="C173" s="1">
         <v>1570</v>
       </c>
@@ -5920,13 +5865,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="174" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B174" s="2">
-        <v>427</v>
-      </c>
       <c r="C174" s="1">
         <v>1100</v>
       </c>
@@ -5937,13 +5879,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="175" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B175" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="C175" s="1">
         <v>2150</v>
       </c>
@@ -5965,6 +5904,15 @@
       <c r="K175" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH175" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK175" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM175" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS175" s="1" t="s">
         <v>209</v>
       </c>
@@ -5977,14 +5925,14 @@
       <c r="BY175" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="176" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD175" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="176" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B176" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="C176" s="1">
         <v>2150</v>
       </c>
@@ -6006,6 +5954,15 @@
       <c r="K176" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH176" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK176" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM176" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS176" s="1" t="s">
         <v>209</v>
       </c>
@@ -6017,15 +5974,15 @@
       </c>
       <c r="BY176" s="1">
         <v>0</v>
+      </c>
+      <c r="CD176" s="1" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="177" spans="1:71" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B177" s="2">
-        <v>476</v>
-      </c>
       <c r="C177" s="1">
         <v>1230</v>
       </c>
@@ -6040,9 +5997,6 @@
       <c r="A178" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B178" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="C178" s="1">
         <v>2150</v>
       </c>
@@ -6057,9 +6011,6 @@
       <c r="A179" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B179" s="2">
-        <v>250</v>
-      </c>
       <c r="C179" s="1">
         <v>2150</v>
       </c>
@@ -6074,9 +6025,6 @@
       <c r="A180" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B180" s="2">
-        <v>283</v>
-      </c>
       <c r="C180" s="1">
         <v>2150</v>
       </c>
@@ -6091,9 +6039,6 @@
       <c r="A181" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B181" s="2">
-        <v>299</v>
-      </c>
       <c r="C181" s="1">
         <v>2150</v>
       </c>
@@ -6108,9 +6053,6 @@
       <c r="A182" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B182" s="2">
-        <v>261</v>
-      </c>
       <c r="C182" s="1">
         <v>2150</v>
       </c>
@@ -6125,9 +6067,6 @@
       <c r="A183" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>248</v>
-      </c>
       <c r="C183" s="1">
         <v>2150</v>
       </c>
@@ -6142,9 +6081,6 @@
       <c r="A184" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B184" s="2">
-        <v>274</v>
-      </c>
       <c r="C184" s="1">
         <v>2150</v>
       </c>
@@ -6159,9 +6095,6 @@
       <c r="A185" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B185" s="2">
-        <v>379</v>
-      </c>
       <c r="C185" s="1">
         <v>1100</v>
       </c>
@@ -6176,9 +6109,6 @@
       <c r="A186" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B186" s="2">
-        <v>181</v>
-      </c>
       <c r="C186" s="1">
         <v>1650</v>
       </c>
@@ -6193,9 +6123,6 @@
       <c r="A187" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B187" s="2">
-        <v>603</v>
-      </c>
       <c r="C187" s="1">
         <v>1250</v>
       </c>
@@ -6210,9 +6137,6 @@
       <c r="A188" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B188" s="2">
-        <v>602</v>
-      </c>
       <c r="C188" s="1">
         <v>1500</v>
       </c>
@@ -6227,9 +6151,6 @@
       <c r="A189" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B189" s="2">
-        <v>167</v>
-      </c>
       <c r="C189" s="1">
         <v>2000</v>
       </c>
@@ -6244,9 +6165,6 @@
       <c r="A190" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B190" s="2">
-        <v>192</v>
-      </c>
       <c r="C190" s="1">
         <v>1400</v>
       </c>
@@ -6261,9 +6179,6 @@
       <c r="A191" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B191" s="2">
-        <v>156</v>
-      </c>
       <c r="C191" s="1">
         <v>1600</v>
       </c>
@@ -6278,9 +6193,6 @@
       <c r="A192" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B192" s="2">
-        <v>511</v>
-      </c>
       <c r="C192" s="1">
         <v>1800</v>
       </c>
@@ -6291,13 +6203,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="193" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B193" s="2">
-        <v>512</v>
-      </c>
       <c r="C193" s="1">
         <v>1800</v>
       </c>
@@ -6308,13 +6217,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="194" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B194" s="2">
-        <v>237</v>
-      </c>
       <c r="C194" s="1">
         <v>2150</v>
       </c>
@@ -6336,6 +6242,15 @@
       <c r="K194" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH194" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK194" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM194" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS194" s="1" t="s">
         <v>209</v>
       </c>
@@ -6348,14 +6263,14 @@
       <c r="BY194" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="195" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD194" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="195" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="C195" s="1">
         <v>2150</v>
       </c>
@@ -6366,13 +6281,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="196" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B196" s="2">
-        <v>112</v>
-      </c>
       <c r="C196" s="1">
         <v>1600</v>
       </c>
@@ -6383,13 +6295,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="197" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="C197" s="1">
         <v>1360</v>
       </c>
@@ -6400,13 +6309,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="198" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B198" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="C198" s="1">
         <v>2150</v>
       </c>
@@ -6417,13 +6323,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B199" s="2">
-        <v>255</v>
-      </c>
       <c r="C199" s="1">
         <v>2150</v>
       </c>
@@ -6434,13 +6337,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="200" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B200" s="2">
-        <v>163</v>
-      </c>
       <c r="C200" s="1">
         <v>1600</v>
       </c>
@@ -6451,13 +6351,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="201" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="C201" s="1">
         <v>2150</v>
       </c>
@@ -6479,6 +6376,15 @@
       <c r="K201" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH201" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK201" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM201" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS201" s="1" t="s">
         <v>209</v>
       </c>
@@ -6491,14 +6397,14 @@
       <c r="BY201" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="202" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD201" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="202" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A202" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B202" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C202" s="1">
         <v>2150</v>
       </c>
@@ -6509,13 +6415,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="203" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A203" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B203" s="2">
-        <v>601</v>
-      </c>
       <c r="C203" s="1">
         <v>1500</v>
       </c>
@@ -6526,13 +6429,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="204" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A204" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B204" s="2">
-        <v>244</v>
-      </c>
       <c r="C204" s="1">
         <v>2150</v>
       </c>
@@ -6543,13 +6443,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="205" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A205" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B205" s="2">
-        <v>238</v>
-      </c>
       <c r="C205" s="1">
         <v>2150</v>
       </c>
@@ -6560,13 +6457,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="206" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A206" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B206" s="2">
-        <v>291</v>
-      </c>
       <c r="C206" s="1">
         <v>2150</v>
       </c>
@@ -6577,13 +6471,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="207" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A207" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B207" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="C207" s="1">
         <v>2150</v>
       </c>
@@ -6594,13 +6485,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="208" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A208" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B208" s="2">
-        <v>508</v>
-      </c>
       <c r="C208" s="1">
         <v>1800</v>
       </c>
@@ -6611,13 +6499,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="209" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A209" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B209" s="2">
-        <v>267</v>
-      </c>
       <c r="C209" s="1">
         <v>445</v>
       </c>
@@ -6628,13 +6513,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="210" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A210" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>255</v>
-      </c>
       <c r="C210" s="1">
         <v>1150</v>
       </c>
@@ -6645,13 +6527,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A211" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B211" s="2">
-        <v>612</v>
-      </c>
       <c r="C211" s="1">
         <v>1600</v>
       </c>
@@ -6662,13 +6541,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A212" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B212" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="C212" s="1">
         <v>2150</v>
       </c>
@@ -6690,6 +6566,15 @@
       <c r="K212" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH212" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK212" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM212" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS212" s="1" t="s">
         <v>209</v>
       </c>
@@ -6702,14 +6587,14 @@
       <c r="BY212" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD212" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="213" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A213" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="C213" s="1">
         <v>2150</v>
       </c>
@@ -6720,13 +6605,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="214" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A214" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B214" s="2">
-        <v>338</v>
-      </c>
       <c r="C214" s="1">
         <v>1600</v>
       </c>
@@ -6737,13 +6619,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="215" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A215" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B215" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="C215" s="1">
         <v>2150</v>
       </c>
@@ -6765,6 +6644,15 @@
       <c r="K215" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH215" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK215" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM215" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS215" s="1" t="s">
         <v>209</v>
       </c>
@@ -6777,14 +6665,14 @@
       <c r="BY215" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="216" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD215" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="216" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A216" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B216" s="2">
-        <v>239</v>
-      </c>
       <c r="C216" s="1">
         <v>2150</v>
       </c>
@@ -6806,6 +6694,15 @@
       <c r="K216" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="AH216" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="BK216" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM216" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="BS216" s="1" t="s">
         <v>209</v>
       </c>
@@ -6818,14 +6715,14 @@
       <c r="BY216" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="217" spans="1:77" x14ac:dyDescent="0.35">
+      <c r="CD216" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A217" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>220</v>
-      </c>
       <c r="C217" s="1">
         <v>2150</v>
       </c>
@@ -6833,13 +6730,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="218" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A218" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B218" s="2">
-        <v>299</v>
-      </c>
       <c r="C218" s="1">
         <v>2150</v>
       </c>
@@ -6847,13 +6741,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="219" spans="1:77" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:82" x14ac:dyDescent="0.35">
       <c r="A219" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B219" s="2">
-        <v>245</v>
-      </c>
       <c r="C219" s="1">
         <v>2150</v>
       </c>
@@ -6861,88 +6752,24 @@
         <v>209</v>
       </c>
     </row>
-    <row r="220" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A220" t="s">
-        <v>260</v>
-      </c>
-      <c r="B220" s="2">
-        <v>526</v>
-      </c>
-      <c r="C220">
-        <v>600</v>
+    <row r="220" spans="1:82" x14ac:dyDescent="0.35">
+      <c r="A220" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="K220" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="221" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A221" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B221" s="2">
-        <v>496</v>
-      </c>
-      <c r="C221">
-        <v>1640</v>
-      </c>
-    </row>
-    <row r="222" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A222" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B222" s="2">
-        <v>179</v>
-      </c>
-      <c r="C222">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="223" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A223" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B223" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C223">
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="224" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A224" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="B224" s="2">
-        <v>503</v>
-      </c>
-      <c r="C224">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A225" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="B225" s="2">
-        <v>138</v>
-      </c>
-      <c r="C225">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A226" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:CX220"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="K3 K4:K220 BS3:BS218" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>